<commit_message>
updating files for paper revision
</commit_message>
<xml_diff>
--- a/miscs/organ_classification_final.xlsx
+++ b/miscs/organ_classification_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jyshoji/Research_data/Hybrida/final_analysis/miscs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020346F0-0C2C-3343-870A-A99A3F319867}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CA0F2A-5E5A-FF4A-84B1-0FBEED024ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3020" yWindow="460" windowWidth="25780" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3020" yWindow="500" windowWidth="25780" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="final3" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="219">
   <si>
     <t>embryonic</t>
   </si>
@@ -646,6 +646,54 @@
   </si>
   <si>
     <t>secondary lymphoid</t>
+  </si>
+  <si>
+    <t>appendix</t>
+  </si>
+  <si>
+    <t>larynx</t>
+  </si>
+  <si>
+    <t>pharynx</t>
+  </si>
+  <si>
+    <t>nasopharynx</t>
+  </si>
+  <si>
+    <t>oropharynx</t>
+  </si>
+  <si>
+    <t>hypopharynx</t>
+  </si>
+  <si>
+    <t>neuromesoderm</t>
+  </si>
+  <si>
+    <t>hindgut</t>
+  </si>
+  <si>
+    <t>autonomic ganglion</t>
+  </si>
+  <si>
+    <t>ventral midbrain</t>
+  </si>
+  <si>
+    <t>meninges</t>
+  </si>
+  <si>
+    <t>enteric nervous system</t>
+  </si>
+  <si>
+    <t>gingival crevice</t>
+  </si>
+  <si>
+    <t>blood-air barrier</t>
+  </si>
+  <si>
+    <t>artificial joint</t>
+  </si>
+  <si>
+    <t>anulus fibrosus</t>
   </si>
 </sst>
 </file>
@@ -710,17 +758,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1035,10 +1078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M141"/>
+  <dimension ref="A1:M152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43:D44"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1051,7 +1094,7 @@
     <col min="6" max="6" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>194</v>
       </c>
@@ -1061,7 +1104,7 @@
       <c r="C1" t="s">
         <v>192</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>181</v>
       </c>
       <c r="E1" t="s">
@@ -1070,61 +1113,50 @@
       <c r="F1" t="s">
         <v>123</v>
       </c>
-      <c r="L1" s="2"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E2" s="8" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
         <v>179</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="H2" s="2"/>
-      <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E3" s="8" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
         <v>173</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D4" s="8" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" t="s">
         <v>178</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D5" s="8"/>
-      <c r="E5" s="8" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
         <v>177</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D6" s="8"/>
-      <c r="E6" s="8" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
         <v>176</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C7" s="8" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
         <v>175</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
         <v>190</v>
       </c>
@@ -1132,938 +1164,890 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="8" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
         <v>171</v>
       </c>
       <c r="C9" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>104</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C11" s="8" t="s">
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
         <v>199</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" t="s">
         <v>193</v>
       </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="8" t="s">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C14" s="2" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D16" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C15" s="2" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
         <v>146</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D17" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B16" s="2" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
         <v>46</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>162</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>164</v>
       </c>
-      <c r="B21" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C25" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
         <v>80</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C28" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C27" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>163</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" t="s">
         <v>25</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C35" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C34" s="2" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
         <v>158</v>
       </c>
-      <c r="D34" s="7"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C35" s="6" t="s">
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B36" s="7"/>
-      <c r="C36" s="6" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B38" s="4"/>
+      <c r="C38" t="s">
         <v>198</v>
       </c>
-      <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B37" s="7"/>
-      <c r="C37" s="6" t="s">
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B39" s="4"/>
+      <c r="C39" t="s">
         <v>115</v>
       </c>
-      <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C40" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C39" s="5" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C41" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B40" s="1" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C42" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C41" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>70</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B46" t="s">
         <v>23</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C46" t="s">
         <v>201</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D46" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D44" t="s">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C45" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
         <v>202</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D48" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D46" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D47" s="2" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D48" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
         <v>127</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E51" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>159</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B54" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
         <v>37</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C56" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C54" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C57" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>26</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B59" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>22</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B62" t="s">
         <v>21</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C62" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C60" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C63" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B61" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
         <v>34</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C64" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C62" t="s">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C65" t="s">
         <v>101</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D65" t="s">
         <v>130</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E65" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D63" t="s">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
         <v>132</v>
       </c>
-      <c r="E63" s="6"/>
-      <c r="F63" s="2"/>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D64" t="s">
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D67" t="s">
         <v>133</v>
       </c>
-      <c r="M64" s="3"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="M67" s="2"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>82</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B69" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B67" t="s">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
         <v>44</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C70" t="s">
+        <v>205</v>
+      </c>
+      <c r="D70" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D71" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D72" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C73" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C74" t="s">
         <v>45</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D74" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B68" t="s">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
         <v>19</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C75" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C69" t="s">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C76" t="s">
         <v>36</v>
       </c>
-      <c r="L69" s="1"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C70" t="s">
+      <c r="L76" s="1"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C77" t="s">
         <v>134</v>
       </c>
-      <c r="L70" s="1"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B71" s="8" t="s">
+      <c r="L77" s="1"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C78" t="s">
+        <v>216</v>
+      </c>
+      <c r="L78" s="1"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B79" t="s">
         <v>167</v>
       </c>
-      <c r="C71" s="9"/>
-      <c r="L71" s="1"/>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="C79" s="4"/>
+      <c r="L79" s="1"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>7</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B81" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B74" s="2" t="s">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B82" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B75" t="s">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B83" t="s">
         <v>9</v>
       </c>
-      <c r="C75" s="8" t="s">
+      <c r="C83" t="s">
         <v>185</v>
       </c>
-      <c r="D75" s="8"/>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C76" s="8" t="s">
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C84" t="s">
         <v>120</v>
       </c>
-      <c r="D76" s="8" t="s">
+      <c r="D84" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C77" s="8" t="s">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C85" t="s">
         <v>119</v>
       </c>
-      <c r="D77" s="8"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C78" s="6" t="s">
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C86" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B79" s="2" t="s">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B87" t="s">
         <v>8</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C87" t="s">
         <v>10</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D87" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D80" t="s">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D88" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D81" t="s">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D89" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C82" t="s">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C90" t="s">
         <v>14</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D90" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D83" t="s">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D91" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D84" t="s">
+      <c r="E91" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D92" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>106</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B94" t="s">
         <v>17</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C94" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C87" t="s">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C95" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B88" t="s">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B96" t="s">
         <v>31</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C96" t="s">
         <v>135</v>
       </c>
-      <c r="D88" s="8" t="s">
+      <c r="D96" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B89" t="s">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
         <v>27</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C97" t="s">
         <v>28</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D97" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D90" t="s">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D98" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C91" t="s">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C99" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="2" t="s">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
         <v>3</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B101" t="s">
         <v>137</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="C101" t="s">
         <v>50</v>
       </c>
-      <c r="D93" s="2"/>
-      <c r="E93" s="2"/>
-      <c r="F93" s="2"/>
-      <c r="G93" s="2"/>
-      <c r="H93" s="2"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="2"/>
-      <c r="B94" s="2"/>
-      <c r="C94" s="2" t="s">
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C102" t="s">
         <v>5</v>
       </c>
-      <c r="D94" s="2"/>
-      <c r="E94" s="2"/>
-      <c r="F94" s="2"/>
-      <c r="G94" s="2"/>
-      <c r="H94" s="2"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" s="2"/>
-      <c r="B95" s="2"/>
-      <c r="C95" s="2" t="s">
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C103" t="s">
         <v>2</v>
       </c>
-      <c r="D95" s="2" t="s">
+      <c r="D103" t="s">
         <v>1</v>
       </c>
-      <c r="E95" s="2" t="s">
+      <c r="E103" t="s">
         <v>90</v>
       </c>
-      <c r="F95" s="2"/>
-      <c r="G95" s="2"/>
-      <c r="H95" s="2"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="2"/>
-      <c r="B96" s="2"/>
-      <c r="C96" s="2"/>
-      <c r="D96" s="2"/>
-      <c r="E96" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F96" s="2"/>
-      <c r="G96" s="2"/>
-      <c r="H96" s="2"/>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A97" s="2"/>
-      <c r="B97" s="2"/>
-      <c r="C97" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D97" s="2"/>
-      <c r="E97" s="2"/>
-      <c r="F97" s="2"/>
-      <c r="G97" s="2"/>
-      <c r="H97" s="2"/>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A98" s="2"/>
-      <c r="B98" s="2"/>
-      <c r="C98" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D98" s="2"/>
-      <c r="E98" s="2"/>
-      <c r="F98" s="2"/>
-      <c r="G98" s="2"/>
-      <c r="H98" s="2"/>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A99" s="2"/>
-      <c r="B99" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D99" s="2"/>
-      <c r="E99" s="2"/>
-      <c r="F99" s="2"/>
-      <c r="G99" s="2"/>
-      <c r="H99" s="2"/>
-      <c r="K99" s="1"/>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A100" s="2"/>
-      <c r="B100" s="2"/>
-      <c r="C100" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D100" s="2"/>
-      <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
-      <c r="G100" s="2"/>
-      <c r="H100" s="2"/>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A101" s="2"/>
-      <c r="B101" s="2"/>
-      <c r="C101" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D101" s="2"/>
-      <c r="E101" s="2"/>
-      <c r="F101" s="2"/>
-      <c r="G101" s="2"/>
-      <c r="H101" s="2"/>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>116</v>
-      </c>
-      <c r="B103" t="s">
-        <v>29</v>
-      </c>
-      <c r="C103" t="s">
-        <v>30</v>
-      </c>
-      <c r="D103" t="s">
-        <v>139</v>
-      </c>
-      <c r="E103" t="s">
-        <v>95</v>
-      </c>
-      <c r="H103" s="2"/>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E104" t="s">
-        <v>140</v>
+        <v>84</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E105" t="s">
-        <v>141</v>
+      <c r="C105" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D106" t="s">
-        <v>142</v>
+      <c r="C106" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
+        <v>152</v>
+      </c>
+      <c r="C107" t="s">
+        <v>13</v>
+      </c>
+      <c r="K107" s="1"/>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C108" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C109" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>116</v>
+      </c>
+      <c r="B111" t="s">
+        <v>29</v>
+      </c>
+      <c r="C111" t="s">
+        <v>30</v>
+      </c>
+      <c r="D111" t="s">
+        <v>139</v>
+      </c>
+      <c r="E111" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E112" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E113" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D114" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B115" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B108" s="1" t="s">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B116" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B109" s="1"/>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B117" s="1"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
         <v>165</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B118" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C110" s="8" t="s">
+      <c r="C118" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C111" s="8" t="s">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C119" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B112" t="s">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B120" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B113" t="s">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B121" t="s">
         <v>118</v>
       </c>
-      <c r="C113" s="1"/>
-      <c r="H113" s="1"/>
-      <c r="J113" s="3"/>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B114" s="1"/>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
+      <c r="C121" s="1"/>
+      <c r="H121" s="1"/>
+      <c r="J121" s="2"/>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B122" s="1"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
         <v>39</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B123" t="s">
         <v>58</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C123" t="s">
         <v>40</v>
       </c>
-      <c r="D115" s="2"/>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C116" t="s">
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C124" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B117" t="s">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B125" t="s">
         <v>76</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C125" t="s">
         <v>72</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D125" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C118" s="6" t="s">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C126" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B119" s="2" t="s">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C127" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B128" t="s">
         <v>66</v>
       </c>
-      <c r="D119" s="2"/>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B120" s="2" t="s">
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B129" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B130" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
         <v>174</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B132" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B125" s="6" t="s">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B133" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B126" s="6"/>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A127" s="2" t="s">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
         <v>157</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B135" t="s">
         <v>0</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C135" t="s">
         <v>200</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D135" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D128" t="s">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D136" t="s">
         <v>196</v>
       </c>
-      <c r="H128" s="1"/>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C129" s="2" t="s">
+      <c r="H136" s="1"/>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C137" t="s">
         <v>197</v>
       </c>
-      <c r="D129" s="2" t="s">
+      <c r="D137" t="s">
         <v>0</v>
       </c>
-      <c r="E129" s="2" t="s">
+      <c r="E137" t="s">
         <v>61</v>
       </c>
-      <c r="F129" s="5" t="s">
+      <c r="F137" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G129" s="2"/>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A130" s="2"/>
-      <c r="C130" s="2"/>
-      <c r="D130" s="2"/>
-      <c r="E130" s="2"/>
-      <c r="F130" s="2" t="s">
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F138" t="s">
         <v>108</v>
       </c>
-      <c r="G130" s="2"/>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A131" s="2"/>
-      <c r="C131" s="2"/>
-      <c r="D131" s="2" t="s">
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D139" t="s">
         <v>155</v>
       </c>
-      <c r="E131" s="2" t="s">
+      <c r="E139" t="s">
         <v>4</v>
       </c>
-      <c r="F131" s="5" t="s">
+      <c r="F139" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G131" s="2"/>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A132" s="2"/>
-      <c r="C132" s="2" t="s">
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C140" t="s">
         <v>154</v>
       </c>
-      <c r="D132" s="2" t="s">
+      <c r="D140" t="s">
         <v>0</v>
       </c>
-      <c r="E132" s="2" t="s">
+      <c r="E140" t="s">
         <v>77</v>
       </c>
-      <c r="F132" s="2" t="s">
+      <c r="F140" t="s">
         <v>97</v>
       </c>
-      <c r="G132" s="2" t="s">
+      <c r="G140" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A133" s="2"/>
-      <c r="C133" s="2"/>
-      <c r="D133" s="2"/>
-      <c r="E133" s="2" t="s">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G141" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E142" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E143" t="s">
         <v>113</v>
       </c>
-      <c r="F133" s="2"/>
-      <c r="G133" s="2"/>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A134" s="2"/>
-      <c r="C134" s="2"/>
-      <c r="D134" s="2"/>
-      <c r="E134" s="2" t="s">
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E144" t="s">
         <v>79</v>
       </c>
-      <c r="F134" s="2"/>
-      <c r="G134" s="2"/>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A135" s="2"/>
-      <c r="C135" s="2"/>
-      <c r="D135" s="2"/>
-      <c r="E135" s="2" t="s">
+    </row>
+    <row r="145" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E145" t="s">
         <v>122</v>
       </c>
-      <c r="F135" s="2"/>
-      <c r="G135" s="2"/>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A136" s="2"/>
-      <c r="C136" s="2"/>
-      <c r="D136" s="2"/>
-      <c r="E136" s="2" t="s">
+    </row>
+    <row r="146" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E146" t="s">
         <v>98</v>
       </c>
-      <c r="F136" s="2"/>
-      <c r="G136" s="2"/>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A137" s="2"/>
-      <c r="C137" s="2"/>
-      <c r="D137" s="2"/>
-      <c r="E137" s="2" t="s">
+    </row>
+    <row r="147" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E147" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="148" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E148" t="s">
         <v>153</v>
       </c>
-      <c r="F137" s="2"/>
-      <c r="G137" s="2"/>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A138" s="2"/>
-      <c r="C138" s="2"/>
-      <c r="D138" s="2"/>
-      <c r="E138" s="2" t="s">
+    </row>
+    <row r="149" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E149" t="s">
         <v>150</v>
       </c>
-      <c r="F138" s="2" t="s">
+      <c r="F149" t="s">
         <v>151</v>
       </c>
-      <c r="G138" s="2"/>
-      <c r="H138" s="2"/>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A139" s="2"/>
-      <c r="C139" s="2"/>
-      <c r="D139" s="2" t="s">
+    </row>
+    <row r="150" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D150" t="s">
         <v>155</v>
       </c>
-      <c r="E139" s="2" t="s">
+      <c r="E150" t="s">
         <v>48</v>
       </c>
-      <c r="F139" s="2" t="s">
+      <c r="F150" t="s">
         <v>138</v>
       </c>
-      <c r="G139" s="2"/>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="2"/>
-      <c r="C140" s="2"/>
-      <c r="D140" s="2"/>
-      <c r="E140" s="2"/>
-      <c r="F140" s="2" t="s">
+    </row>
+    <row r="151" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F151" t="s">
         <v>148</v>
       </c>
-      <c r="G140" s="2" t="s">
+      <c r="G151" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B141" t="s">
+    <row r="152" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B152" t="s">
         <v>156</v>
       </c>
     </row>

</xml_diff>